<commit_message>
updated plots and form
</commit_message>
<xml_diff>
--- a/data/Dismantling.xlsx
+++ b/data/Dismantling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2FBDE7-D7B4-45E7-ABF5-5479FFDD3F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2874E5-815C-4437-A00E-27FCB2A00986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{7AF44DFD-6DE0-425B-8A1D-E2D48A19D1FC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
     <sheet name="Comment" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1323,8 +1323,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638B28E4-B6D3-44B6-9A21-CAA5A049F06A}">
   <dimension ref="A1:EW61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EQ11" workbookViewId="0">
-      <selection activeCell="EY53" sqref="EY53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="DP20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="EY58" sqref="EY58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5021,457 +5024,457 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AE9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AH9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AK9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AL9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AM9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AN9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AO9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AP9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AQ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AR9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AS9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AT9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AU9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AV9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AW9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AX9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AY9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AZ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BA9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BB9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BC9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BD9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BE9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BF9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BG9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BH9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BI9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BJ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BK9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BL9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BM9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BN9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BO9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BQ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BR9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BS9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BT9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BU9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BV9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BW9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BX9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BY9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BZ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CA9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CB9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CC9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CD9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CE9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CF9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CG9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CH9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CI9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CJ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CK9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CL9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CM9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CN9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CO9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CP9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CQ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CR9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CS9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CT9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CU9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CV9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CW9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CX9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CY9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CZ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DA9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DB9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DC9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DD9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DE9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DF9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DG9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DH9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DI9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DJ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DK9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DL9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DM9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DN9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DO9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DP9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DQ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DR9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DS9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DT9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DU9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DV9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DW9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DX9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DY9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DZ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EA9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EB9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EC9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ED9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EE9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EF9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EG9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EH9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EI9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EJ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EK9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EL9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EM9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EN9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EO9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EP9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EQ9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ER9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ES9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ET9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EU9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EV9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EW9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.25">
@@ -7225,97 +7228,97 @@
         <v>0</v>
       </c>
       <c r="DS13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DT13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DU13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DV13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DW13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DX13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DY13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DZ13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EA13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EB13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EC13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ED13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EE13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EF13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EG13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EH13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EI13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EJ13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EK13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EL13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EM13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EN13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EO13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EP13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EQ13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ER13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ES13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ET13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EU13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EV13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EW13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="1:153" x14ac:dyDescent="0.25">
@@ -10553,457 +10556,457 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AA21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AB21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AE21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AF21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AG21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AH21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AI21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AK21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AL21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AM21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AN21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AO21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AP21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AQ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AR21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AS21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AT21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AU21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AV21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AW21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AX21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AY21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AZ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BA21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BB21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BC21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BD21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BE21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BF21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BG21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BH21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BI21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BJ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BK21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BL21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BM21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BN21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BO21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BQ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BR21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BS21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BT21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BU21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BV21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BW21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BX21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BY21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BZ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CA21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CB21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CC21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CD21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CE21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CF21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CG21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CH21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CI21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CJ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CK21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CL21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CM21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CN21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CO21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CP21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CQ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CR21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CS21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CT21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CU21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CV21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CW21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CX21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CY21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CZ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DA21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DB21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DC21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DD21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DE21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DF21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DG21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DH21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DI21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DJ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DK21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DL21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DM21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DN21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DO21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DP21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DQ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DR21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DS21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DT21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DU21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DV21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DW21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DX21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DY21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DZ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EA21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EB21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EC21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ED21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EE21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EF21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EG21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EH21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EI21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EJ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EK21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EL21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EM21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EN21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EO21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EP21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EQ21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ER21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ES21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ET21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EU21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EV21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EW21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="22" spans="1:153" x14ac:dyDescent="0.25">
@@ -12757,97 +12760,97 @@
         <v>0</v>
       </c>
       <c r="DS25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DT25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DU25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DV25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DW25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DX25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DY25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DZ25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EA25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EB25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EC25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ED25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EE25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EF25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EG25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EH25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EI25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EJ25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EK25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EL25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EM25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EN25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EO25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EP25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EQ25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ER25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ES25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ET25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EU25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EV25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EW25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:153" x14ac:dyDescent="0.25">
@@ -16085,457 +16088,457 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="O33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="V33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="W33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="X33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Y33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Z33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AA33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AB33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AE33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AF33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AG33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AH33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AI33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AK33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AL33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AM33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AN33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AO33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AP33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AQ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AR33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AS33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AT33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AU33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AV33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AW33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AX33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AY33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AZ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BA33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BB33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BC33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BD33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BE33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BF33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BG33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BH33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BI33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BJ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BK33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BL33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BM33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BN33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BO33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BQ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BR33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BS33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BT33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BU33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BV33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BW33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BX33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BY33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BZ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CA33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CB33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CC33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CD33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CE33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CF33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CG33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CH33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CI33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CJ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CK33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CL33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CM33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CN33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CO33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CP33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CQ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CR33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CS33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CT33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CU33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CV33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CW33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CX33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CY33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CZ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DA33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DB33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DC33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DD33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DE33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DF33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DG33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DH33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DI33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DJ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DK33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DL33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DM33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DN33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DO33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DP33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DQ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DR33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DS33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DT33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DU33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DV33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DW33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DX33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DY33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DZ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EA33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EB33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EC33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ED33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EE33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EF33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EG33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EH33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EI33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EJ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EK33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EL33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EM33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EN33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EO33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EP33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EQ33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ER33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ES33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ET33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EU33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EV33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EW33">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="34" spans="1:153" x14ac:dyDescent="0.25">
@@ -18289,97 +18292,97 @@
         <v>0</v>
       </c>
       <c r="DS37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DT37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DU37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DV37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DW37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DX37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DY37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DZ37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EA37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EB37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EC37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ED37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EE37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EF37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EG37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EH37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EI37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EJ37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EK37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EL37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EM37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EN37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EO37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EP37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EQ37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ER37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ES37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ET37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EU37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EV37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EW37">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:153" x14ac:dyDescent="0.25">
@@ -21617,457 +21620,457 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="O45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="V45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="W45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="X45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Y45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Z45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AA45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AB45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AE45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AF45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AG45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AH45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AI45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AK45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AL45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AM45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AN45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AO45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AP45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AQ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AR45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AS45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AT45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AU45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AV45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AW45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AX45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AY45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AZ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BA45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BB45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BC45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BD45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BE45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BF45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BG45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BH45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BI45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BJ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BK45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BL45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BM45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BN45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BO45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BQ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BR45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BS45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BT45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BU45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BV45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BW45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BX45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BY45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BZ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CA45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CB45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CC45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CD45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CE45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CF45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CG45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CH45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CI45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CJ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CK45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CL45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CM45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CN45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CO45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CP45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CQ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CR45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CS45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CT45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CU45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CV45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CW45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CX45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CY45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CZ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DA45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DB45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DC45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DD45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DE45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DF45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DG45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DH45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DI45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DJ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DK45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DL45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DM45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DN45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DO45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DP45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DQ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DR45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DS45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DT45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DU45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DV45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DW45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DX45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DY45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DZ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EA45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EB45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EC45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ED45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EE45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EF45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EG45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EH45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EI45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EJ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EK45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EL45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EM45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EN45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EO45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EP45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EQ45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ER45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ES45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ET45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EU45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EV45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EW45">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="46" spans="1:153" x14ac:dyDescent="0.25">
@@ -23821,97 +23824,97 @@
         <v>0</v>
       </c>
       <c r="DS49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DT49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DU49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DV49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DW49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DX49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DY49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="DZ49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EA49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EB49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EC49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ED49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EE49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EF49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EG49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EH49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EI49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EJ49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EK49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EL49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EM49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EN49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EO49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EP49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EQ49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ER49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ES49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="ET49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EU49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EV49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EW49">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:153" x14ac:dyDescent="0.25">
@@ -27149,457 +27152,457 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="R57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="T57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="U57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="V57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="W57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="X57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Y57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Z57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AA57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AB57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AE57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AF57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AG57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AH57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AI57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AK57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AL57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AM57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AN57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AO57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AP57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AQ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AR57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AS57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AT57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AU57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AV57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AW57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AX57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AY57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AZ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BA57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BB57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BC57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BD57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BE57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BF57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BG57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BH57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BI57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BJ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BK57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BL57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BM57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BN57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BO57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BQ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BR57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BS57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BT57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BU57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BV57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BW57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BX57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BY57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BZ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CA57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CB57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CC57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CD57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CE57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CF57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CG57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CH57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CI57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CJ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CK57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CL57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CM57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CN57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CO57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CP57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CQ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CR57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CS57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CT57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CU57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CV57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CW57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CX57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CY57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="CZ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DA57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DB57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DC57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DD57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DE57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DF57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DG57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DH57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DI57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DJ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DK57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DL57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DM57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DN57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DO57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DP57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DQ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DR57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DS57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DT57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DU57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DV57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DW57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DX57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DY57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="DZ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EA57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EB57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EC57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ED57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EE57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EF57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EG57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EH57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EI57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EJ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EK57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EL57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EM57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EN57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EO57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EP57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EQ57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ER57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ES57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="ET57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EU57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EV57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="EW57">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="58" spans="1:153" x14ac:dyDescent="0.25">
@@ -29353,97 +29356,97 @@
         <v>0</v>
       </c>
       <c r="DS61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DT61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DU61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DV61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DW61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DX61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DY61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="DZ61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EA61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EB61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EC61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ED61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EE61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EF61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EG61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EH61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EI61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EJ61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EK61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EL61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EM61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EN61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EO61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EP61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EQ61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ER61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ES61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="ET61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EU61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EV61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EW61">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>